<commit_message>
adicionando genero e corrigindo artistas
</commit_message>
<xml_diff>
--- a/base_musical.xlsx
+++ b/base_musical.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="151">
   <si>
     <t>artista</t>
   </si>
@@ -55,120 +55,144 @@
     <t>duracao_ms</t>
   </si>
   <si>
-    <t>Bizarrap</t>
+    <t>genero</t>
+  </si>
+  <si>
+    <t>Bizarrap, Quevedo</t>
   </si>
   <si>
     <t>Harry Styles</t>
   </si>
   <si>
+    <t>Bad Bunny, Chencho Corleone</t>
+  </si>
+  <si>
     <t>Bad Bunny</t>
   </si>
   <si>
+    <t>ROSALÍA</t>
+  </si>
+  <si>
     <t>BLACKPINK</t>
   </si>
   <si>
-    <t>ROSALÍA</t>
-  </si>
-  <si>
     <t>Manuel Turizo</t>
   </si>
   <si>
+    <t>OneRepublic</t>
+  </si>
+  <si>
+    <t>David Guetta, Bebe Rexha</t>
+  </si>
+  <si>
     <t>Kate Bush</t>
   </si>
   <si>
+    <t>Bad Bunny, Bomba Estéreo</t>
+  </si>
+  <si>
+    <t>Chris Brown</t>
+  </si>
+  <si>
+    <t>Nicki Minaj</t>
+  </si>
+  <si>
+    <t>Steve Lacy</t>
+  </si>
+  <si>
     <t>Joji</t>
   </si>
   <si>
-    <t>OneRepublic</t>
-  </si>
-  <si>
-    <t>Steve Lacy</t>
-  </si>
-  <si>
-    <t>Chris Brown</t>
-  </si>
-  <si>
     <t>Glass Animals</t>
   </si>
   <si>
     <t>KAROL G</t>
   </si>
   <si>
-    <t>Charlie Puth</t>
-  </si>
-  <si>
-    <t>Nicki Minaj</t>
-  </si>
-  <si>
     <t>Rosa Linn</t>
   </si>
   <si>
-    <t>The Kid LAROI</t>
+    <t>Central Cee</t>
+  </si>
+  <si>
+    <t>Charlie Puth, Jung Kook, BTS</t>
+  </si>
+  <si>
+    <t>The Kid LAROI, Justin Bieber</t>
+  </si>
+  <si>
+    <t>Elton John, Britney Spears</t>
   </si>
   <si>
     <t>Tom Odell</t>
   </si>
   <si>
-    <t>Central Cee</t>
-  </si>
-  <si>
-    <t>Elton John</t>
+    <t>Lizzo</t>
+  </si>
+  <si>
+    <t>Post Malone, Doja Cat</t>
   </si>
   <si>
     <t>Stephen Sanchez</t>
   </si>
   <si>
-    <t>Lizzo</t>
-  </si>
-  <si>
-    <t>Nicky Youre</t>
-  </si>
-  <si>
-    <t>Post Malone</t>
+    <t>KAROL G, Maldy</t>
+  </si>
+  <si>
+    <t>Nicky Youre, dazy</t>
+  </si>
+  <si>
+    <t>James Hype, Miggy Dela Rosa</t>
+  </si>
+  <si>
+    <t>Luar La L</t>
+  </si>
+  <si>
+    <t>Bad Bunny, Jhay Cortez</t>
+  </si>
+  <si>
+    <t>Elton John, Dua Lipa, PNAU</t>
+  </si>
+  <si>
+    <t>Shakira, Rauw Alejandro</t>
+  </si>
+  <si>
+    <t>Imagine Dragons</t>
+  </si>
+  <si>
+    <t>Drake, 21 Savage</t>
+  </si>
+  <si>
+    <t>Bad Bunny, Rauw Alejandro</t>
   </si>
   <si>
     <t>The Weeknd</t>
   </si>
   <si>
-    <t>Shakira</t>
+    <t>Camila Cabello, Ed Sheeran</t>
   </si>
   <si>
     <t>The Neighbourhood</t>
   </si>
   <si>
-    <t>Luar La L</t>
-  </si>
-  <si>
-    <t>James Hype</t>
-  </si>
-  <si>
-    <t>David Guetta</t>
-  </si>
-  <si>
-    <t>IVE</t>
-  </si>
-  <si>
     <t>Rels B</t>
   </si>
   <si>
-    <t>Camila Cabello</t>
-  </si>
-  <si>
-    <t>benny blanco</t>
-  </si>
-  <si>
-    <t>Drake</t>
-  </si>
-  <si>
-    <t>Imagine Dragons</t>
-  </si>
-  <si>
     <t>Ghost</t>
   </si>
   <si>
+    <t>Doja Cat</t>
+  </si>
+  <si>
+    <t>Gorillaz, Tame Impala, Bootie Brown</t>
+  </si>
+  <si>
     <t>Justin Bieber</t>
   </si>
   <si>
+    <t>Rauw Alejandro, Lyanno, Brray</t>
+  </si>
+  <si>
     <t>Quevedo: Bzrp Music Sessions, Vol. 52</t>
   </si>
   <si>
@@ -181,16 +205,22 @@
     <t>Tití Me Preguntó</t>
   </si>
   <si>
+    <t>DESPECHÁ</t>
+  </si>
+  <si>
     <t>Pink Venom</t>
   </si>
   <si>
-    <t>DESPECHÁ</t>
+    <t>La Bachata</t>
   </si>
   <si>
     <t>Efecto</t>
   </si>
   <si>
-    <t>La Bachata</t>
+    <t>I Ain't Worried</t>
+  </si>
+  <si>
+    <t>I'm Good (Blue)</t>
   </si>
   <si>
     <t>Running Up That Hill (A Deal With God)</t>
@@ -199,121 +229,244 @@
     <t>Ojitos Lindos</t>
   </si>
   <si>
+    <t>Under The Influence</t>
+  </si>
+  <si>
+    <t>Super Freaky Girl</t>
+  </si>
+  <si>
+    <t>Bad Habit</t>
+  </si>
+  <si>
     <t>Glimpse of Us</t>
   </si>
   <si>
-    <t>I Ain't Worried</t>
-  </si>
-  <si>
-    <t>Bad Habit</t>
-  </si>
-  <si>
     <t>Moscow Mule</t>
   </si>
   <si>
-    <t>Under The Influence</t>
-  </si>
-  <si>
     <t>Heat Waves</t>
   </si>
   <si>
     <t>PROVENZA</t>
   </si>
   <si>
+    <t>SNAP</t>
+  </si>
+  <si>
+    <t>Doja</t>
+  </si>
+  <si>
     <t>Left and Right (Feat. Jung Kook of BTS)</t>
   </si>
   <si>
-    <t>Super Freaky Girl</t>
-  </si>
-  <si>
-    <t>SNAP</t>
+    <t>Late Night Talking</t>
   </si>
   <si>
     <t>STAY (with Justin Bieber)</t>
   </si>
   <si>
+    <t>Hold Me Closer</t>
+  </si>
+  <si>
     <t>Another Love</t>
   </si>
   <si>
-    <t>Doja</t>
+    <t>About Damn Time</t>
+  </si>
+  <si>
+    <t>I Like You (A Happier Song) (with Doja Cat)</t>
   </si>
   <si>
     <t>Neverita</t>
   </si>
   <si>
-    <t>Late Night Talking</t>
+    <t>Until I Found You</t>
+  </si>
+  <si>
+    <t>GATÚBELA</t>
+  </si>
+  <si>
+    <t>Sunroof</t>
+  </si>
+  <si>
+    <t>Ferrari</t>
+  </si>
+  <si>
+    <t>Caile</t>
+  </si>
+  <si>
+    <t>Tarot</t>
   </si>
   <si>
     <t>Cold Heart - PNAU Remix</t>
   </si>
   <si>
-    <t>Until I Found You</t>
-  </si>
-  <si>
-    <t>Tarot</t>
-  </si>
-  <si>
-    <t>About Damn Time</t>
-  </si>
-  <si>
-    <t>Sunroof</t>
-  </si>
-  <si>
-    <t>I Like You (A Happier Song) (with Doja Cat)</t>
-  </si>
-  <si>
-    <t>Hold Me Closer</t>
+    <t>Te Felicito</t>
+  </si>
+  <si>
+    <t>Bones</t>
+  </si>
+  <si>
+    <t>Jimmy Cooks (feat. 21 Savage)</t>
+  </si>
+  <si>
+    <t>Party</t>
   </si>
   <si>
     <t>Die For You</t>
   </si>
   <si>
-    <t>Te Felicito</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>GATÚBELA</t>
+    <t>Bam Bam (feat. Ed Sheeran)</t>
   </si>
   <si>
     <t>Sweater Weather</t>
   </si>
   <si>
-    <t>Caile</t>
-  </si>
-  <si>
-    <t>Ferrari</t>
-  </si>
-  <si>
-    <t>I'm Good (Blue)</t>
-  </si>
-  <si>
-    <t>After LIKE</t>
-  </si>
-  <si>
     <t>cómo dormiste?</t>
   </si>
   <si>
-    <t>Bam Bam (feat. Ed Sheeran)</t>
-  </si>
-  <si>
-    <t>Bad Decisions (with BTS &amp; Snoop Dogg)</t>
-  </si>
-  <si>
-    <t>Jimmy Cooks (feat. 21 Savage)</t>
+    <t>Mary On A Cross</t>
+  </si>
+  <si>
+    <t>Vegas (From the Original Motion Picture Soundtrack ELVIS)</t>
+  </si>
+  <si>
+    <t>New Gold (feat. Tame Impala and Bootie Brown)</t>
+  </si>
+  <si>
+    <t>LOKERA</t>
   </si>
   <si>
     <t>Blinding Lights</t>
   </si>
   <si>
-    <t>Bones</t>
-  </si>
-  <si>
-    <t>Mary On A Cross</t>
-  </si>
-  <si>
-    <t>La Corriente</t>
+    <t>argentine hip hop, pop venezolano, trap argentino, rap canario, trap latino</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latin, reggaeton, trap latino, </t>
+  </si>
+  <si>
+    <t>latin, reggaeton, trap latino</t>
+  </si>
+  <si>
+    <t>r&amp;b en espanol</t>
+  </si>
+  <si>
+    <t>k-pop, k-pop girl group</t>
+  </si>
+  <si>
+    <t>colombian pop, latin, reggaeton, reggaeton colombiano, trap latino</t>
+  </si>
+  <si>
+    <t>dance pop, piano rock, pop, pop rock</t>
+  </si>
+  <si>
+    <t>big room, dance pop, edm, pop, pop dance, pop rap, dance pop, electropop, pop, post-teen pop, uk pop</t>
+  </si>
+  <si>
+    <t>art pop, art rock, baroque pop, new wave pop, permanent wave, piano rock, singer-songwriter</t>
+  </si>
+  <si>
+    <t>latin, reggaeton, trap latino, cumbia, latin alternative, pop electronico, tropical alternativo</t>
+  </si>
+  <si>
+    <t>dance pop, pop, pop rap, r&amp;b</t>
+  </si>
+  <si>
+    <t>dance pop, hip pop, pop, queens hip hop, rap</t>
+  </si>
+  <si>
+    <t>afrofuturism</t>
+  </si>
+  <si>
+    <t>viral pop</t>
+  </si>
+  <si>
+    <t>gauze pop, indietronica, shiver pop</t>
+  </si>
+  <si>
+    <t>latin, reggaeton, reggaeton colombiano</t>
+  </si>
+  <si>
+    <t>drill brasileiro</t>
+  </si>
+  <si>
+    <t>dance pop, pop, viral pop, , k-pop, k-pop boy group</t>
+  </si>
+  <si>
+    <t>australian hip hop, pop, canadian pop, pop</t>
+  </si>
+  <si>
+    <t>glam rock, mellow gold, piano rock, dance pop, pop, post-teen pop</t>
+  </si>
+  <si>
+    <t>chill pop, pop</t>
+  </si>
+  <si>
+    <t>dance pop, escape room, minnesota hip hop, pop, trap queen</t>
+  </si>
+  <si>
+    <t>dfw rap, melodic rap, rap, dance pop, pop</t>
+  </si>
+  <si>
+    <t>gen z singer-songwriter, pop</t>
+  </si>
+  <si>
+    <t>latin, reggaeton, reggaeton colombiano, latin hip hop, perreo, reggaeton, reggaeton flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">deep groove house, edm, house, pop dance, tropical house, uk dance, </t>
+  </si>
+  <si>
+    <t>reggaeton, reggaeton flow, trap latino</t>
+  </si>
+  <si>
+    <t>latin, reggaeton, trap latino, latin, reggaeton, trap latino</t>
+  </si>
+  <si>
+    <t>glam rock, mellow gold, piano rock, dance pop, pop, uk pop, alternative dance, aussietronica, australian dance, australian electropop</t>
+  </si>
+  <si>
+    <t>colombian pop, dance pop, latin, latin pop, puerto rican pop, trap latino</t>
+  </si>
+  <si>
+    <t>modern rock, rock</t>
+  </si>
+  <si>
+    <t>canadian hip hop, canadian pop, hip hop, pop, rap, toronto rap, atl hip hop, rap, trap</t>
+  </si>
+  <si>
+    <t>latin, reggaeton, trap latino, puerto rican pop, trap latino</t>
+  </si>
+  <si>
+    <t>canadian contemporary r&amp;b, canadian pop, pop</t>
+  </si>
+  <si>
+    <t>dance pop, pop, post-teen pop, uk pop, pop, uk pop</t>
+  </si>
+  <si>
+    <t>modern alternative rock, modern rock, pop, shimmer pop</t>
+  </si>
+  <si>
+    <t>r&amp;b en espanol, spanish hip hop, trap latino, urbano espanol</t>
+  </si>
+  <si>
+    <t>hard rock, metal</t>
+  </si>
+  <si>
+    <t>dance pop, pop</t>
+  </si>
+  <si>
+    <t>canadian pop, pop</t>
+  </si>
+  <si>
+    <t>puerto rican pop, trap latino, latin, latin hip hop, reggaeton, reggaeton flow, trap boricua, trap latino, reggaeton, reggaeton flow, trap latino</t>
   </si>
 </sst>
 </file>
@@ -671,13 +824,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,16 +870,19 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D2">
         <v>0.621</v>
@@ -761,16 +917,19 @@
       <c r="N2">
         <v>198938</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>0.52</v>
@@ -805,16 +964,19 @@
       <c r="N3">
         <v>167303</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>0.911</v>
@@ -849,16 +1011,19 @@
       <c r="N4">
         <v>178567</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>0.65</v>
@@ -893,676 +1058,724 @@
       <c r="N5">
         <v>243717</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D6">
-        <v>0.798</v>
+        <v>0.919</v>
       </c>
       <c r="E6">
-        <v>0.697</v>
+        <v>0.623</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>-7.139</v>
+        <v>-6.521</v>
       </c>
       <c r="H6">
-        <v>0.0891</v>
+        <v>0.0992</v>
       </c>
       <c r="I6">
-        <v>0.0202</v>
+        <v>0.184</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1.63E-05</v>
       </c>
       <c r="K6">
-        <v>0.259</v>
+        <v>0.0609</v>
       </c>
       <c r="L6">
-        <v>0.745</v>
+        <v>0.775</v>
       </c>
       <c r="M6">
-        <v>90.03100000000001</v>
+        <v>130.037</v>
       </c>
       <c r="N6">
-        <v>186964</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>157018</v>
+      </c>
+      <c r="O6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D7">
-        <v>0.919</v>
+        <v>0.798</v>
       </c>
       <c r="E7">
-        <v>0.623</v>
+        <v>0.697</v>
       </c>
       <c r="F7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>-6.521</v>
+        <v>-7.139</v>
       </c>
       <c r="H7">
-        <v>0.0992</v>
+        <v>0.0891</v>
       </c>
       <c r="I7">
-        <v>0.184</v>
+        <v>0.0202</v>
       </c>
       <c r="J7">
-        <v>1.63E-05</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>0.0609</v>
+        <v>0.259</v>
       </c>
       <c r="L7">
-        <v>0.775</v>
+        <v>0.745</v>
       </c>
       <c r="M7">
-        <v>130.037</v>
+        <v>90.03100000000001</v>
       </c>
       <c r="N7">
-        <v>157018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>186964</v>
+      </c>
+      <c r="O7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D8">
-        <v>0.801</v>
+        <v>0.835</v>
       </c>
       <c r="E8">
-        <v>0.475</v>
+        <v>0.679</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
       <c r="G8">
-        <v>-8.797000000000001</v>
+        <v>-5.329</v>
       </c>
       <c r="H8">
-        <v>0.0516</v>
+        <v>0.0364</v>
       </c>
       <c r="I8">
-        <v>0.141</v>
+        <v>0.583</v>
       </c>
       <c r="J8">
-        <v>1.73E-05</v>
+        <v>1.98E-06</v>
       </c>
       <c r="K8">
-        <v>0.0639</v>
+        <v>0.218</v>
       </c>
       <c r="L8">
-        <v>0.234</v>
+        <v>0.85</v>
       </c>
       <c r="M8">
-        <v>98.047</v>
+        <v>124.98</v>
       </c>
       <c r="N8">
-        <v>213061</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>162638</v>
+      </c>
+      <c r="O8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D9">
-        <v>0.835</v>
+        <v>0.801</v>
       </c>
       <c r="E9">
-        <v>0.679</v>
+        <v>0.475</v>
       </c>
       <c r="F9">
         <v>7</v>
       </c>
       <c r="G9">
-        <v>-5.329</v>
+        <v>-8.797000000000001</v>
       </c>
       <c r="H9">
-        <v>0.0364</v>
+        <v>0.0516</v>
       </c>
       <c r="I9">
-        <v>0.583</v>
+        <v>0.141</v>
       </c>
       <c r="J9">
-        <v>1.98E-06</v>
+        <v>1.73E-05</v>
       </c>
       <c r="K9">
-        <v>0.218</v>
+        <v>0.0639</v>
       </c>
       <c r="L9">
-        <v>0.85</v>
+        <v>0.234</v>
       </c>
       <c r="M9">
-        <v>124.98</v>
+        <v>98.047</v>
       </c>
       <c r="N9">
-        <v>162638</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>213061</v>
+      </c>
+      <c r="O9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D10">
-        <v>0.629</v>
+        <v>0.704</v>
       </c>
       <c r="E10">
-        <v>0.547</v>
+        <v>0.797</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>-13.123</v>
+        <v>-5.927</v>
       </c>
       <c r="H10">
-        <v>0.055</v>
+        <v>0.0475</v>
       </c>
       <c r="I10">
-        <v>0.72</v>
+        <v>0.08260000000000001</v>
       </c>
       <c r="J10">
-        <v>0.00314</v>
+        <v>0.000745</v>
       </c>
       <c r="K10">
-        <v>0.0604</v>
+        <v>0.0546</v>
       </c>
       <c r="L10">
-        <v>0.197</v>
+        <v>0.825</v>
       </c>
       <c r="M10">
-        <v>108.375</v>
+        <v>139.994</v>
       </c>
       <c r="N10">
-        <v>298933</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>148486</v>
+      </c>
+      <c r="O10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D11">
-        <v>0.647</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="E11">
-        <v>0.6860000000000001</v>
+        <v>0.965</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G11">
-        <v>-5.745</v>
+        <v>-3.673</v>
       </c>
       <c r="H11">
-        <v>0.0413</v>
+        <v>0.0343</v>
       </c>
       <c r="I11">
-        <v>0.08</v>
+        <v>0.00383</v>
       </c>
       <c r="J11">
-        <v>1.34E-06</v>
+        <v>7.07E-06</v>
       </c>
       <c r="K11">
-        <v>0.528</v>
+        <v>0.371</v>
       </c>
       <c r="L11">
-        <v>0.268</v>
+        <v>0.304</v>
       </c>
       <c r="M11">
-        <v>79.928</v>
+        <v>128.04</v>
       </c>
       <c r="N11">
-        <v>258299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>175238</v>
+      </c>
+      <c r="O11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D12">
-        <v>0.44</v>
+        <v>0.629</v>
       </c>
       <c r="E12">
-        <v>0.317</v>
+        <v>0.547</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G12">
-        <v>-9.257999999999999</v>
+        <v>-13.123</v>
       </c>
       <c r="H12">
-        <v>0.0531</v>
+        <v>0.055</v>
       </c>
       <c r="I12">
-        <v>0.891</v>
+        <v>0.72</v>
       </c>
       <c r="J12">
-        <v>4.78E-06</v>
+        <v>0.00314</v>
       </c>
       <c r="K12">
-        <v>0.141</v>
+        <v>0.0604</v>
       </c>
       <c r="L12">
-        <v>0.268</v>
+        <v>0.197</v>
       </c>
       <c r="M12">
-        <v>169.914</v>
+        <v>108.375</v>
       </c>
       <c r="N12">
-        <v>233456</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>298933</v>
+      </c>
+      <c r="O12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D13">
-        <v>0.704</v>
+        <v>0.647</v>
       </c>
       <c r="E13">
-        <v>0.797</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>-5.927</v>
+        <v>-5.745</v>
       </c>
       <c r="H13">
-        <v>0.0475</v>
+        <v>0.0413</v>
       </c>
       <c r="I13">
-        <v>0.08260000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="J13">
-        <v>0.000745</v>
+        <v>1.34E-06</v>
       </c>
       <c r="K13">
-        <v>0.0546</v>
+        <v>0.528</v>
       </c>
       <c r="L13">
-        <v>0.825</v>
+        <v>0.268</v>
       </c>
       <c r="M13">
-        <v>139.994</v>
+        <v>79.928</v>
       </c>
       <c r="N13">
-        <v>148486</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>258299</v>
+      </c>
+      <c r="O13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D14">
-        <v>0.6860000000000001</v>
+        <v>0.733</v>
       </c>
       <c r="E14">
-        <v>0.494</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>-7.093</v>
+        <v>-5.529</v>
       </c>
       <c r="H14">
-        <v>0.0355</v>
+        <v>0.0427</v>
       </c>
       <c r="I14">
-        <v>0.613</v>
+        <v>0.0635</v>
       </c>
       <c r="J14">
-        <v>5.8E-05</v>
+        <v>1.18E-06</v>
       </c>
       <c r="K14">
-        <v>0.402</v>
+        <v>0.105</v>
       </c>
       <c r="L14">
-        <v>0.7</v>
+        <v>0.31</v>
       </c>
       <c r="M14">
-        <v>168.946</v>
+        <v>116.992</v>
       </c>
       <c r="N14">
-        <v>232067</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>184613</v>
+      </c>
+      <c r="O14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D15">
-        <v>0.804</v>
+        <v>0.951</v>
       </c>
       <c r="E15">
-        <v>0.674</v>
+        <v>0.878</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>-5.453</v>
+        <v>-2.565</v>
       </c>
       <c r="H15">
-        <v>0.0333</v>
+        <v>0.211</v>
       </c>
       <c r="I15">
-        <v>0.294</v>
+        <v>0.0509</v>
       </c>
       <c r="J15">
-        <v>1.18E-06</v>
+        <v>1.61E-05</v>
       </c>
       <c r="K15">
-        <v>0.115</v>
+        <v>0.321</v>
       </c>
       <c r="L15">
-        <v>0.292</v>
+        <v>0.923</v>
       </c>
       <c r="M15">
-        <v>99.968</v>
+        <v>133.014</v>
       </c>
       <c r="N15">
-        <v>245940</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>170977</v>
+      </c>
+      <c r="O15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D16">
-        <v>0.733</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="E16">
-        <v>0.6899999999999999</v>
+        <v>0.494</v>
       </c>
       <c r="F16">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>-5.529</v>
+        <v>-7.093</v>
       </c>
       <c r="H16">
-        <v>0.0427</v>
+        <v>0.0355</v>
       </c>
       <c r="I16">
-        <v>0.0635</v>
+        <v>0.613</v>
       </c>
       <c r="J16">
-        <v>1.18E-06</v>
+        <v>5.8E-05</v>
       </c>
       <c r="K16">
-        <v>0.105</v>
+        <v>0.402</v>
       </c>
       <c r="L16">
-        <v>0.31</v>
+        <v>0.7</v>
       </c>
       <c r="M16">
-        <v>116.992</v>
+        <v>168.946</v>
       </c>
       <c r="N16">
-        <v>184613</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>232067</v>
+      </c>
+      <c r="O16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D17">
-        <v>0.761</v>
+        <v>0.44</v>
       </c>
       <c r="E17">
-        <v>0.525</v>
+        <v>0.317</v>
       </c>
       <c r="F17">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>-6.9</v>
+        <v>-9.257999999999999</v>
       </c>
       <c r="H17">
-        <v>0.0944</v>
+        <v>0.0531</v>
       </c>
       <c r="I17">
-        <v>0.44</v>
+        <v>0.891</v>
       </c>
       <c r="J17">
-        <v>6.7E-06</v>
+        <v>4.78E-06</v>
       </c>
       <c r="K17">
-        <v>0.0921</v>
+        <v>0.141</v>
       </c>
       <c r="L17">
-        <v>0.531</v>
+        <v>0.268</v>
       </c>
       <c r="M17">
-        <v>80.87</v>
+        <v>169.914</v>
       </c>
       <c r="N17">
-        <v>238805</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>233456</v>
+      </c>
+      <c r="O17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D18">
-        <v>0.87</v>
+        <v>0.804</v>
       </c>
       <c r="E18">
-        <v>0.516</v>
+        <v>0.674</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G18">
-        <v>-8.006</v>
+        <v>-5.453</v>
       </c>
       <c r="H18">
-        <v>0.0541</v>
+        <v>0.0333</v>
       </c>
       <c r="I18">
-        <v>0.656</v>
+        <v>0.294</v>
       </c>
       <c r="J18">
-        <v>0.008229999999999999</v>
+        <v>1.18E-06</v>
       </c>
       <c r="K18">
-        <v>0.11</v>
+        <v>0.115</v>
       </c>
       <c r="L18">
-        <v>0.53</v>
+        <v>0.292</v>
       </c>
       <c r="M18">
-        <v>111.005</v>
+        <v>99.968</v>
       </c>
       <c r="N18">
-        <v>210200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>245940</v>
+      </c>
+      <c r="O18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D19">
-        <v>0.881</v>
+        <v>0.761</v>
       </c>
       <c r="E19">
-        <v>0.592</v>
+        <v>0.525</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>-4.898</v>
+        <v>-6.9</v>
       </c>
       <c r="H19">
-        <v>0.0324</v>
+        <v>0.0944</v>
       </c>
       <c r="I19">
-        <v>0.619</v>
+        <v>0.44</v>
       </c>
       <c r="J19">
-        <v>1.32E-05</v>
+        <v>6.7E-06</v>
       </c>
       <c r="K19">
-        <v>0.0901</v>
+        <v>0.0921</v>
       </c>
       <c r="L19">
-        <v>0.719</v>
+        <v>0.531</v>
       </c>
       <c r="M19">
-        <v>101.058</v>
+        <v>80.87</v>
       </c>
       <c r="N19">
-        <v>154487</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>238805</v>
+      </c>
+      <c r="O19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D20">
-        <v>0.951</v>
+        <v>0.87</v>
       </c>
       <c r="E20">
-        <v>0.878</v>
+        <v>0.516</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>-2.565</v>
+        <v>-8.006</v>
       </c>
       <c r="H20">
-        <v>0.211</v>
+        <v>0.0541</v>
       </c>
       <c r="I20">
-        <v>0.0509</v>
+        <v>0.656</v>
       </c>
       <c r="J20">
-        <v>1.61E-05</v>
+        <v>0.008229999999999999</v>
       </c>
       <c r="K20">
-        <v>0.321</v>
+        <v>0.11</v>
       </c>
       <c r="L20">
-        <v>0.923</v>
+        <v>0.53</v>
       </c>
       <c r="M20">
-        <v>133.014</v>
+        <v>111.005</v>
       </c>
       <c r="N20">
-        <v>170977</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>210200</v>
+      </c>
+      <c r="O20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D21">
         <v>0.5649999999999999</v>
@@ -1598,1283 +1811,1334 @@
         <v>179551</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D22">
-        <v>0.591</v>
+        <v>0.911</v>
       </c>
       <c r="E22">
-        <v>0.764</v>
+        <v>0.573</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G22">
-        <v>-5.484</v>
+        <v>-7.43</v>
       </c>
       <c r="H22">
-        <v>0.0483</v>
+        <v>0.288</v>
       </c>
       <c r="I22">
-        <v>0.0383</v>
+        <v>0.38</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0.103</v>
+        <v>0.403</v>
       </c>
       <c r="L22">
-        <v>0.478</v>
+        <v>0.972</v>
       </c>
       <c r="M22">
-        <v>169.928</v>
+        <v>140.04</v>
       </c>
       <c r="N22">
-        <v>141806</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>97393</v>
+      </c>
+      <c r="O22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D23">
-        <v>0.442</v>
+        <v>0.881</v>
       </c>
       <c r="E23">
-        <v>0.538</v>
+        <v>0.592</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G23">
-        <v>-8.550000000000001</v>
+        <v>-4.898</v>
       </c>
       <c r="H23">
-        <v>0.0451</v>
+        <v>0.0324</v>
       </c>
       <c r="I23">
-        <v>0.717</v>
+        <v>0.619</v>
       </c>
       <c r="J23">
-        <v>2.95E-05</v>
+        <v>1.32E-05</v>
       </c>
       <c r="K23">
-        <v>0.09</v>
+        <v>0.0901</v>
       </c>
       <c r="L23">
-        <v>0.139</v>
+        <v>0.719</v>
       </c>
       <c r="M23">
-        <v>122.758</v>
+        <v>101.058</v>
       </c>
       <c r="N23">
-        <v>244360</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>154487</v>
+      </c>
+      <c r="O23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D24">
-        <v>0.911</v>
+        <v>0.714</v>
       </c>
       <c r="E24">
-        <v>0.573</v>
+        <v>0.728</v>
       </c>
       <c r="F24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G24">
-        <v>-7.43</v>
+        <v>-4.595</v>
       </c>
       <c r="H24">
-        <v>0.288</v>
+        <v>0.0468</v>
       </c>
       <c r="I24">
-        <v>0.38</v>
+        <v>0.298</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>0.403</v>
+        <v>0.106</v>
       </c>
       <c r="L24">
-        <v>0.972</v>
+        <v>0.901</v>
       </c>
       <c r="M24">
-        <v>140.04</v>
+        <v>114.996</v>
       </c>
       <c r="N24">
-        <v>97393</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>177955</v>
+      </c>
+      <c r="O24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D25">
-        <v>0.876</v>
+        <v>0.591</v>
       </c>
       <c r="E25">
-        <v>0.498</v>
+        <v>0.764</v>
       </c>
       <c r="F25">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>-7.511</v>
+        <v>-5.484</v>
       </c>
       <c r="H25">
-        <v>0.0478</v>
+        <v>0.0483</v>
       </c>
       <c r="I25">
-        <v>0.0706</v>
+        <v>0.0383</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0.143</v>
+        <v>0.103</v>
       </c>
       <c r="L25">
-        <v>0.428</v>
+        <v>0.478</v>
       </c>
       <c r="M25">
-        <v>122.016</v>
+        <v>169.928</v>
       </c>
       <c r="N25">
-        <v>173119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>141806</v>
+      </c>
+      <c r="O25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D26">
-        <v>0.714</v>
+        <v>0.659</v>
       </c>
       <c r="E26">
-        <v>0.728</v>
+        <v>0.772</v>
       </c>
       <c r="F26">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>-4.595</v>
       </c>
       <c r="H26">
-        <v>0.0468</v>
+        <v>0.11</v>
       </c>
       <c r="I26">
-        <v>0.298</v>
+        <v>0.07480000000000001</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>0.000346</v>
       </c>
       <c r="K26">
-        <v>0.106</v>
+        <v>0.187</v>
       </c>
       <c r="L26">
-        <v>0.901</v>
+        <v>0.484</v>
       </c>
       <c r="M26">
-        <v>114.996</v>
+        <v>126.018</v>
       </c>
       <c r="N26">
-        <v>177955</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>202246</v>
+      </c>
+      <c r="O26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D27">
-        <v>0.795</v>
+        <v>0.442</v>
       </c>
       <c r="E27">
-        <v>0.8</v>
+        <v>0.538</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>-6.32</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="H27">
-        <v>0.0309</v>
+        <v>0.0451</v>
       </c>
       <c r="I27">
-        <v>0.0354</v>
+        <v>0.717</v>
       </c>
       <c r="J27">
-        <v>7.25E-05</v>
+        <v>2.95E-05</v>
       </c>
       <c r="K27">
-        <v>0.0915</v>
+        <v>0.09</v>
       </c>
       <c r="L27">
-        <v>0.9340000000000001</v>
+        <v>0.139</v>
       </c>
       <c r="M27">
-        <v>116.032</v>
+        <v>122.758</v>
       </c>
       <c r="N27">
-        <v>202735</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>244360</v>
+      </c>
+      <c r="O27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D28">
-        <v>0.346</v>
+        <v>0.836</v>
       </c>
       <c r="E28">
-        <v>0.5</v>
+        <v>0.743</v>
       </c>
       <c r="F28">
         <v>10</v>
       </c>
       <c r="G28">
-        <v>-6.097</v>
+        <v>-6.305</v>
       </c>
       <c r="H28">
-        <v>0.0388</v>
+        <v>0.0653</v>
       </c>
       <c r="I28">
-        <v>0.757</v>
+        <v>0.0974</v>
       </c>
       <c r="J28">
         <v>0</v>
       </c>
       <c r="K28">
-        <v>0.189</v>
+        <v>0.335</v>
       </c>
       <c r="L28">
-        <v>0.191</v>
+        <v>0.723</v>
       </c>
       <c r="M28">
-        <v>202.466</v>
+        <v>108.965</v>
       </c>
       <c r="N28">
-        <v>176667</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>191938</v>
+      </c>
+      <c r="O28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D29">
-        <v>0.795</v>
+        <v>0.733</v>
       </c>
       <c r="E29">
-        <v>0.6840000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="F29">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G29">
-        <v>-3.971</v>
+        <v>-6.009</v>
       </c>
       <c r="H29">
-        <v>0.0419</v>
+        <v>0.0751</v>
       </c>
       <c r="I29">
-        <v>0.0225</v>
+        <v>0.121</v>
       </c>
       <c r="J29">
         <v>0</v>
       </c>
       <c r="K29">
-        <v>0.658</v>
+        <v>0.121</v>
       </c>
       <c r="L29">
-        <v>0.419</v>
+        <v>0.472</v>
       </c>
       <c r="M29">
-        <v>114.011</v>
+        <v>100.964</v>
       </c>
       <c r="N29">
-        <v>237895</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>192841</v>
+      </c>
+      <c r="O29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D30">
-        <v>0.836</v>
+        <v>0.876</v>
       </c>
       <c r="E30">
-        <v>0.743</v>
+        <v>0.498</v>
       </c>
       <c r="F30">
         <v>10</v>
       </c>
       <c r="G30">
-        <v>-6.305</v>
+        <v>-7.511</v>
       </c>
       <c r="H30">
-        <v>0.0653</v>
+        <v>0.0478</v>
       </c>
       <c r="I30">
-        <v>0.0974</v>
+        <v>0.0706</v>
       </c>
       <c r="J30">
         <v>0</v>
       </c>
       <c r="K30">
-        <v>0.335</v>
+        <v>0.143</v>
       </c>
       <c r="L30">
-        <v>0.723</v>
+        <v>0.428</v>
       </c>
       <c r="M30">
-        <v>108.965</v>
+        <v>122.016</v>
       </c>
       <c r="N30">
-        <v>191938</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>173119</v>
+      </c>
+      <c r="O30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D31">
-        <v>0.768</v>
+        <v>0.346</v>
       </c>
       <c r="E31">
-        <v>0.714</v>
+        <v>0.5</v>
       </c>
       <c r="F31">
         <v>10</v>
       </c>
       <c r="G31">
-        <v>-5.11</v>
+        <v>-6.097</v>
       </c>
       <c r="H31">
-        <v>0.0401</v>
+        <v>0.0388</v>
       </c>
       <c r="I31">
-        <v>0.352</v>
+        <v>0.757</v>
       </c>
       <c r="J31">
         <v>0</v>
       </c>
       <c r="K31">
-        <v>0.15</v>
+        <v>0.189</v>
       </c>
       <c r="L31">
-        <v>0.842</v>
+        <v>0.191</v>
       </c>
       <c r="M31">
-        <v>131.443</v>
+        <v>202.466</v>
       </c>
       <c r="N31">
-        <v>163026</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>176667</v>
+      </c>
+      <c r="O31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D32">
-        <v>0.733</v>
+        <v>0.627</v>
       </c>
       <c r="E32">
-        <v>0.67</v>
+        <v>0.858</v>
       </c>
       <c r="F32">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G32">
-        <v>-6.009</v>
+        <v>-2.824</v>
       </c>
       <c r="H32">
-        <v>0.0751</v>
+        <v>0.386</v>
       </c>
       <c r="I32">
-        <v>0.121</v>
+        <v>0.263</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
       <c r="K32">
-        <v>0.121</v>
+        <v>0.21</v>
       </c>
       <c r="L32">
-        <v>0.472</v>
+        <v>0.342</v>
       </c>
       <c r="M32">
-        <v>100.964</v>
+        <v>92.523</v>
       </c>
       <c r="N32">
-        <v>192841</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>209160</v>
+      </c>
+      <c r="O32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D33">
-        <v>0.667</v>
+        <v>0.768</v>
       </c>
       <c r="E33">
-        <v>0.75</v>
+        <v>0.714</v>
       </c>
       <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>-5.11</v>
+      </c>
+      <c r="H33">
+        <v>0.0401</v>
+      </c>
+      <c r="I33">
+        <v>0.352</v>
+      </c>
+      <c r="J33">
         <v>0</v>
       </c>
-      <c r="G33">
-        <v>-4.602</v>
-      </c>
-      <c r="H33">
-        <v>0.0906</v>
-      </c>
-      <c r="I33">
-        <v>0.0746</v>
-      </c>
-      <c r="J33">
-        <v>0.000198</v>
-      </c>
       <c r="K33">
-        <v>0.197</v>
+        <v>0.15</v>
       </c>
       <c r="L33">
-        <v>0.486</v>
+        <v>0.842</v>
       </c>
       <c r="M33">
-        <v>126.041</v>
+        <v>131.443</v>
       </c>
       <c r="N33">
-        <v>202246</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>163026</v>
+      </c>
+      <c r="O33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D34">
-        <v>0.586</v>
+        <v>0.847</v>
       </c>
       <c r="E34">
-        <v>0.525</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34">
-        <v>-7.163</v>
+        <v>-7.877</v>
       </c>
       <c r="H34">
-        <v>0.0615</v>
+        <v>0.0493</v>
       </c>
       <c r="I34">
-        <v>0.111</v>
+        <v>0.0127</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>6E-05</v>
       </c>
       <c r="K34">
-        <v>0.134</v>
+        <v>0.0526</v>
       </c>
       <c r="L34">
-        <v>0.508</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="M34">
-        <v>133.629</v>
+        <v>125.004</v>
       </c>
       <c r="N34">
-        <v>260253</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>186662</v>
+      </c>
+      <c r="O34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D35">
-        <v>0.695</v>
+        <v>0.704</v>
       </c>
       <c r="E35">
-        <v>0.636</v>
+        <v>0.756</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>-4.654</v>
+        <v>-4.948</v>
       </c>
       <c r="H35">
-        <v>0.317</v>
+        <v>0.448</v>
       </c>
       <c r="I35">
-        <v>0.234</v>
+        <v>0.298</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>3.75E-06</v>
       </c>
       <c r="K35">
-        <v>0.081</v>
+        <v>0.0852</v>
       </c>
       <c r="L35">
-        <v>0.575</v>
+        <v>0.461</v>
       </c>
       <c r="M35">
-        <v>174.14</v>
+        <v>121.737</v>
       </c>
       <c r="N35">
-        <v>172235</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>141340</v>
+      </c>
+      <c r="O35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D36">
-        <v>0.829</v>
+        <v>0.795</v>
       </c>
       <c r="E36">
-        <v>0.799</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="F36">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G36">
-        <v>-5.389</v>
+        <v>-3.971</v>
       </c>
       <c r="H36">
-        <v>0.0897</v>
+        <v>0.0419</v>
       </c>
       <c r="I36">
-        <v>0.0151</v>
+        <v>0.0225</v>
       </c>
       <c r="J36">
-        <v>0.000543</v>
+        <v>0</v>
       </c>
       <c r="K36">
-        <v>0.242</v>
+        <v>0.658</v>
       </c>
       <c r="L36">
-        <v>0.471</v>
+        <v>0.419</v>
       </c>
       <c r="M36">
-        <v>97.01300000000001</v>
+        <v>114.011</v>
       </c>
       <c r="N36">
-        <v>227629</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>237895</v>
+      </c>
+      <c r="O36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D37">
-        <v>0.627</v>
+        <v>0.795</v>
       </c>
       <c r="E37">
-        <v>0.858</v>
+        <v>0.8</v>
       </c>
       <c r="F37">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>-2.824</v>
+        <v>-6.32</v>
       </c>
       <c r="H37">
-        <v>0.386</v>
+        <v>0.0309</v>
       </c>
       <c r="I37">
-        <v>0.263</v>
+        <v>0.0354</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>7.25E-05</v>
       </c>
       <c r="K37">
-        <v>0.21</v>
+        <v>0.0915</v>
       </c>
       <c r="L37">
-        <v>0.342</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="M37">
-        <v>92.523</v>
+        <v>116.032</v>
       </c>
       <c r="N37">
-        <v>209160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>202735</v>
+      </c>
+      <c r="O37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D38">
-        <v>0.612</v>
+        <v>0.695</v>
       </c>
       <c r="E38">
-        <v>0.8070000000000001</v>
+        <v>0.636</v>
       </c>
       <c r="F38">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G38">
-        <v>-2.81</v>
+        <v>-4.654</v>
       </c>
       <c r="H38">
-        <v>0.0336</v>
+        <v>0.317</v>
       </c>
       <c r="I38">
-        <v>0.0495</v>
+        <v>0.234</v>
       </c>
       <c r="J38">
-        <v>0.0177</v>
+        <v>0</v>
       </c>
       <c r="K38">
-        <v>0.101</v>
+        <v>0.081</v>
       </c>
       <c r="L38">
-        <v>0.398</v>
+        <v>0.575</v>
       </c>
       <c r="M38">
-        <v>124.053</v>
+        <v>174.14</v>
       </c>
       <c r="N38">
-        <v>240400</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>172235</v>
+      </c>
+      <c r="O38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D39">
-        <v>0.704</v>
+        <v>0.772</v>
       </c>
       <c r="E39">
-        <v>0.756</v>
+        <v>0.75</v>
       </c>
       <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <v>-3.67</v>
+      </c>
+      <c r="H39">
+        <v>0.0455</v>
+      </c>
+      <c r="I39">
+        <v>0.0201</v>
+      </c>
+      <c r="J39">
         <v>0</v>
       </c>
-      <c r="G39">
-        <v>-4.948</v>
-      </c>
-      <c r="H39">
-        <v>0.448</v>
-      </c>
-      <c r="I39">
-        <v>0.298</v>
-      </c>
-      <c r="J39">
-        <v>3.75E-06</v>
-      </c>
       <c r="K39">
-        <v>0.0852</v>
+        <v>0.074</v>
       </c>
       <c r="L39">
-        <v>0.461</v>
+        <v>0.587</v>
       </c>
       <c r="M39">
-        <v>121.737</v>
+        <v>114.061</v>
       </c>
       <c r="N39">
-        <v>141340</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>165265</v>
+      </c>
+      <c r="O39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D40">
-        <v>0.847</v>
+        <v>0.529</v>
       </c>
       <c r="E40">
-        <v>0.6899999999999999</v>
+        <v>0.673</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>-7.877</v>
+        <v>-4.711</v>
       </c>
       <c r="H40">
-        <v>0.0493</v>
+        <v>0.175</v>
       </c>
       <c r="I40">
-        <v>0.0127</v>
+        <v>0.000307</v>
       </c>
       <c r="J40">
-        <v>6E-05</v>
+        <v>2.41E-06</v>
       </c>
       <c r="K40">
-        <v>0.0526</v>
+        <v>0.093</v>
       </c>
       <c r="L40">
-        <v>0.6919999999999999</v>
+        <v>0.366</v>
       </c>
       <c r="M40">
-        <v>125.004</v>
+        <v>165.921</v>
       </c>
       <c r="N40">
-        <v>186662</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>218365</v>
+      </c>
+      <c r="O40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D41">
-        <v>0.5610000000000001</v>
+        <v>0.829</v>
       </c>
       <c r="E41">
-        <v>0.965</v>
+        <v>0.799</v>
       </c>
       <c r="F41">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>-3.673</v>
+        <v>-5.389</v>
       </c>
       <c r="H41">
-        <v>0.0343</v>
+        <v>0.0897</v>
       </c>
       <c r="I41">
-        <v>0.00383</v>
+        <v>0.0151</v>
       </c>
       <c r="J41">
-        <v>7.07E-06</v>
+        <v>0.000543</v>
       </c>
       <c r="K41">
-        <v>0.371</v>
+        <v>0.242</v>
       </c>
       <c r="L41">
-        <v>0.304</v>
+        <v>0.471</v>
       </c>
       <c r="M41">
-        <v>128.04</v>
+        <v>97.01300000000001</v>
       </c>
       <c r="N41">
-        <v>175238</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>227629</v>
+      </c>
+      <c r="O41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D42">
-        <v>0.68</v>
+        <v>0.586</v>
       </c>
       <c r="E42">
-        <v>0.922</v>
+        <v>0.525</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>-1.215</v>
+        <v>-7.163</v>
       </c>
       <c r="H42">
-        <v>0.121</v>
+        <v>0.0615</v>
       </c>
       <c r="I42">
-        <v>0.103</v>
+        <v>0.111</v>
       </c>
       <c r="J42">
         <v>0</v>
       </c>
       <c r="K42">
-        <v>0.0877</v>
+        <v>0.134</v>
       </c>
       <c r="L42">
-        <v>0.799</v>
+        <v>0.508</v>
       </c>
       <c r="M42">
-        <v>125.014</v>
+        <v>133.629</v>
       </c>
       <c r="N42">
-        <v>176973</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>260253</v>
+      </c>
+      <c r="O42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D43">
-        <v>0.627</v>
+        <v>0.756</v>
       </c>
       <c r="E43">
-        <v>0.429</v>
+        <v>0.697</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G43">
-        <v>-8.255000000000001</v>
+        <v>-6.377</v>
       </c>
       <c r="H43">
-        <v>0.234</v>
+        <v>0.0401</v>
       </c>
       <c r="I43">
-        <v>0.238</v>
+        <v>0.182</v>
       </c>
       <c r="J43">
         <v>0</v>
       </c>
       <c r="K43">
-        <v>0.122</v>
+        <v>0.333</v>
       </c>
       <c r="L43">
-        <v>0.5649999999999999</v>
+        <v>0.956</v>
       </c>
       <c r="M43">
-        <v>126.426</v>
+        <v>94.996</v>
       </c>
       <c r="N43">
-        <v>112572</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>206071</v>
+      </c>
+      <c r="O43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D44">
-        <v>0.756</v>
+        <v>0.612</v>
       </c>
       <c r="E44">
-        <v>0.697</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="F44">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G44">
-        <v>-6.377</v>
+        <v>-2.81</v>
       </c>
       <c r="H44">
-        <v>0.0401</v>
+        <v>0.0336</v>
       </c>
       <c r="I44">
-        <v>0.182</v>
+        <v>0.0495</v>
       </c>
       <c r="J44">
-        <v>0</v>
+        <v>0.0177</v>
       </c>
       <c r="K44">
-        <v>0.333</v>
+        <v>0.101</v>
       </c>
       <c r="L44">
-        <v>0.956</v>
+        <v>0.398</v>
       </c>
       <c r="M44">
-        <v>94.996</v>
+        <v>124.053</v>
       </c>
       <c r="N44">
-        <v>206071</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>240400</v>
+      </c>
+      <c r="O44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D45">
-        <v>0.762</v>
+        <v>0.627</v>
       </c>
       <c r="E45">
-        <v>0.861</v>
+        <v>0.429</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>-3.296</v>
+        <v>-8.255000000000001</v>
       </c>
       <c r="H45">
-        <v>0.0955</v>
+        <v>0.234</v>
       </c>
       <c r="I45">
-        <v>0.0185</v>
+        <v>0.238</v>
       </c>
       <c r="J45">
         <v>0</v>
       </c>
       <c r="K45">
-        <v>0.264</v>
+        <v>0.122</v>
       </c>
       <c r="L45">
-        <v>0.955</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="M45">
-        <v>120.048</v>
+        <v>126.426</v>
       </c>
       <c r="N45">
-        <v>172714</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>112572</v>
+      </c>
+      <c r="O45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D46">
-        <v>0.529</v>
+        <v>0.466</v>
       </c>
       <c r="E46">
-        <v>0.673</v>
+        <v>0.9</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G46">
-        <v>-4.711</v>
+        <v>-4.469</v>
       </c>
       <c r="H46">
-        <v>0.175</v>
+        <v>0.0447</v>
       </c>
       <c r="I46">
-        <v>0.000307</v>
+        <v>0.000235</v>
       </c>
       <c r="J46">
-        <v>2.41E-06</v>
+        <v>0.00104</v>
       </c>
       <c r="K46">
-        <v>0.093</v>
+        <v>0.103</v>
       </c>
       <c r="L46">
-        <v>0.366</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="M46">
-        <v>165.921</v>
+        <v>130.02</v>
       </c>
       <c r="N46">
-        <v>218365</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>244804</v>
+      </c>
+      <c r="O46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D47">
-        <v>0.514</v>
+        <v>0.801</v>
       </c>
       <c r="E47">
-        <v>0.73</v>
+        <v>0.601</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G47">
-        <v>-5.934</v>
+        <v>-7.574</v>
       </c>
       <c r="H47">
-        <v>0.0598</v>
+        <v>0.255</v>
       </c>
       <c r="I47">
-        <v>0.00146</v>
+        <v>0.07770000000000001</v>
       </c>
       <c r="J47">
-        <v>9.54E-05</v>
+        <v>3.23E-05</v>
       </c>
       <c r="K47">
-        <v>0.0897</v>
+        <v>0.145</v>
       </c>
       <c r="L47">
-        <v>0.334</v>
+        <v>0.74</v>
       </c>
       <c r="M47">
-        <v>171.005</v>
+        <v>159.969</v>
       </c>
       <c r="N47">
-        <v>200040</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>182907</v>
+      </c>
+      <c r="O47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48">
-        <v>0.772</v>
-      </c>
-      <c r="E48">
-        <v>0.75</v>
-      </c>
-      <c r="F48">
-        <v>5</v>
-      </c>
-      <c r="G48">
-        <v>-3.67</v>
-      </c>
-      <c r="H48">
-        <v>0.0455</v>
-      </c>
-      <c r="I48">
-        <v>0.0201</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>0.074</v>
-      </c>
-      <c r="L48">
-        <v>0.587</v>
-      </c>
-      <c r="M48">
-        <v>114.061</v>
-      </c>
-      <c r="N48">
-        <v>165265</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="D49">
-        <v>0.466</v>
+        <v>0.601</v>
       </c>
       <c r="E49">
-        <v>0.9</v>
+        <v>0.741</v>
       </c>
       <c r="F49">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G49">
-        <v>-4.469</v>
+        <v>-5.569</v>
       </c>
       <c r="H49">
-        <v>0.0447</v>
+        <v>0.0478</v>
       </c>
       <c r="I49">
-        <v>0.000235</v>
+        <v>0.185</v>
       </c>
       <c r="J49">
-        <v>0.00104</v>
+        <v>2.91E-05</v>
       </c>
       <c r="K49">
-        <v>0.103</v>
+        <v>0.415</v>
       </c>
       <c r="L49">
-        <v>0.5610000000000001</v>
+        <v>0.441</v>
       </c>
       <c r="M49">
-        <v>130.02</v>
+        <v>153.96</v>
       </c>
       <c r="N49">
-        <v>244804</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>153190</v>
+      </c>
+      <c r="O49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D50">
-        <v>0.663</v>
+        <v>0.834</v>
       </c>
       <c r="E50">
-        <v>0.786</v>
+        <v>0.828</v>
       </c>
       <c r="F50">
         <v>11</v>
       </c>
       <c r="G50">
-        <v>-3.51</v>
+        <v>-2.657</v>
       </c>
       <c r="H50">
-        <v>0.195</v>
+        <v>0.0452</v>
       </c>
       <c r="I50">
-        <v>0.229</v>
+        <v>0.21</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>5.91E-06</v>
       </c>
       <c r="K50">
-        <v>0.219</v>
+        <v>0.103</v>
       </c>
       <c r="L50">
-        <v>0.579</v>
+        <v>0.58</v>
       </c>
       <c r="M50">
-        <v>196.12</v>
+        <v>102.019</v>
       </c>
       <c r="N50">
-        <v>198367</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <v>195294</v>
+      </c>
+      <c r="O50" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2882,40 +3146,43 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="D51">
-        <v>0.601</v>
+        <v>0.514</v>
       </c>
       <c r="E51">
-        <v>0.741</v>
+        <v>0.73</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G51">
-        <v>-5.569</v>
+        <v>-5.934</v>
       </c>
       <c r="H51">
-        <v>0.0478</v>
+        <v>0.0598</v>
       </c>
       <c r="I51">
-        <v>0.185</v>
+        <v>0.00146</v>
       </c>
       <c r="J51">
-        <v>2.91E-05</v>
+        <v>9.54E-05</v>
       </c>
       <c r="K51">
-        <v>0.415</v>
+        <v>0.0897</v>
       </c>
       <c r="L51">
-        <v>0.441</v>
+        <v>0.334</v>
       </c>
       <c r="M51">
-        <v>153.96</v>
+        <v>171.005</v>
       </c>
       <c r="N51">
-        <v>153190</v>
+        <v>200040</v>
+      </c>
+      <c r="O51" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>